<commit_message>
GB Reduced data fuel type updated with SVCs
</commit_message>
<xml_diff>
--- a/OATS-testcases/GB_ReducedNetwork.xlsx
+++ b/OATS-testcases/GB_ReducedNetwork.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="673">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1774,6 +1774,9 @@
   </si>
   <si>
     <t xml:space="preserve">G3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVC</t>
   </si>
   <si>
     <t xml:space="preserve">G4</t>
@@ -2215,7 +2218,7 @@
   <dimension ref="A1:K137"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A119" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I17:I55 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="Q10 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7037,7 +7040,7 @@
   <dimension ref="B1:AL1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="1" sqref="I17:I55 N21"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="1" sqref="Q10 N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7120,7 +7123,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="I17:I55 J24"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="Q10 J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7133,7 +7136,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7157,7 +7160,7 @@
   <dimension ref="A1:E136"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E87" activeCellId="1" sqref="I17:I55 E87"/>
+      <selection pane="topLeft" activeCell="E87" activeCellId="1" sqref="Q10 E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9314,7 +9317,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I17:I55 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="Q10 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10556,7 +10559,7 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O14" activeCellId="1" sqref="I17:I55 O14"/>
+      <selection pane="topLeft" activeCell="O14" activeCellId="1" sqref="Q10 O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15588,7 +15591,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="1" sqref="I17:I55 A93"/>
+      <selection pane="topLeft" activeCell="A93" activeCellId="1" sqref="Q10 A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20787,7 +20790,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="I17:I55 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="Q10 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20857,7 +20860,7 @@
   <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I17:I55"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="1" sqref="Q10 I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22482,7 +22485,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I17:I55 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="Q10 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22527,7 +22530,7 @@
   <dimension ref="A1:Z84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17:I55"/>
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22827,7 +22830,7 @@
         <v>2</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>364</v>
@@ -22865,7 +22868,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>149</v>
@@ -22907,7 +22910,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>364</v>
@@ -22945,7 +22948,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>149</v>
@@ -22987,7 +22990,7 @@
         <v>2</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R6" s="0" t="s">
         <v>364</v>
@@ -23025,7 +23028,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>149</v>
@@ -23067,7 +23070,7 @@
         <v>2</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R7" s="0" t="s">
         <v>364</v>
@@ -23105,7 +23108,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>149</v>
@@ -23147,7 +23150,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R8" s="0" t="s">
         <v>364</v>
@@ -23185,7 +23188,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>149</v>
@@ -23227,7 +23230,7 @@
         <v>2</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R9" s="0" t="s">
         <v>364</v>
@@ -23265,7 +23268,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>149</v>
@@ -23307,7 +23310,7 @@
         <v>2</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R10" s="0" t="s">
         <v>364</v>
@@ -23345,7 +23348,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>149</v>
@@ -23387,7 +23390,7 @@
         <v>2</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R11" s="0" t="s">
         <v>364</v>
@@ -23425,7 +23428,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>149</v>
@@ -23467,7 +23470,7 @@
         <v>2</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R12" s="0" t="s">
         <v>364</v>
@@ -23505,7 +23508,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>149</v>
@@ -23547,7 +23550,7 @@
         <v>2</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R13" s="0" t="s">
         <v>364</v>
@@ -23585,7 +23588,7 @@
         <v>45</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>149</v>
@@ -23627,7 +23630,7 @@
         <v>2</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="R14" s="0" t="s">
         <v>364</v>
@@ -23665,7 +23668,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>149</v>
@@ -23707,7 +23710,7 @@
         <v>2</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R15" s="0" t="s">
         <v>364</v>
@@ -23745,7 +23748,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>149</v>
@@ -23787,7 +23790,7 @@
         <v>2</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R16" s="0" t="s">
         <v>364</v>
@@ -23825,7 +23828,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>149</v>
@@ -23867,7 +23870,7 @@
         <v>2</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>364</v>
@@ -23905,7 +23908,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>149</v>
@@ -23947,7 +23950,7 @@
         <v>2</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="R18" s="0" t="s">
         <v>364</v>
@@ -23985,7 +23988,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>149</v>
@@ -24027,7 +24030,7 @@
         <v>2</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R19" s="0" t="s">
         <v>364</v>
@@ -24065,7 +24068,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>149</v>
@@ -24107,7 +24110,7 @@
         <v>2</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R20" s="0" t="s">
         <v>364</v>
@@ -24145,7 +24148,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>149</v>
@@ -24187,7 +24190,7 @@
         <v>2</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R21" s="0" t="s">
         <v>364</v>
@@ -24225,7 +24228,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>149</v>
@@ -24267,7 +24270,7 @@
         <v>2</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R22" s="0" t="s">
         <v>364</v>
@@ -24305,7 +24308,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>149</v>
@@ -24347,7 +24350,7 @@
         <v>2</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R23" s="0" t="s">
         <v>364</v>
@@ -24385,7 +24388,7 @@
         <v>56</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>149</v>
@@ -24427,7 +24430,7 @@
         <v>2</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R24" s="0" t="s">
         <v>364</v>
@@ -24465,7 +24468,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>149</v>
@@ -24507,7 +24510,7 @@
         <v>2</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R25" s="0" t="s">
         <v>364</v>
@@ -24545,7 +24548,7 @@
         <v>58</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>149</v>
@@ -24587,7 +24590,7 @@
         <v>2</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R26" s="0" t="s">
         <v>364</v>
@@ -24625,7 +24628,7 @@
         <v>59</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>149</v>
@@ -24667,7 +24670,7 @@
         <v>2</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R27" s="0" t="s">
         <v>364</v>
@@ -24705,7 +24708,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>149</v>
@@ -24747,7 +24750,7 @@
         <v>2</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R28" s="0" t="s">
         <v>364</v>
@@ -24785,7 +24788,7 @@
         <v>62</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>149</v>
@@ -24827,7 +24830,7 @@
         <v>2</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R29" s="0" t="s">
         <v>364</v>
@@ -24865,7 +24868,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>149</v>
@@ -24907,7 +24910,7 @@
         <v>2</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R30" s="0" t="s">
         <v>364</v>
@@ -24945,7 +24948,7 @@
         <v>65</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>149</v>
@@ -24987,7 +24990,7 @@
         <v>2</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R31" s="0" t="s">
         <v>364</v>
@@ -25025,7 +25028,7 @@
         <v>66</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>149</v>
@@ -25067,7 +25070,7 @@
         <v>2</v>
       </c>
       <c r="Q32" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R32" s="0" t="s">
         <v>364</v>
@@ -25105,7 +25108,7 @@
         <v>67</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>149</v>
@@ -25147,7 +25150,7 @@
         <v>2</v>
       </c>
       <c r="Q33" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="R33" s="0" t="s">
         <v>364</v>
@@ -25185,7 +25188,7 @@
         <v>68</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>149</v>
@@ -25227,7 +25230,7 @@
         <v>2</v>
       </c>
       <c r="Q34" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R34" s="0" t="s">
         <v>364</v>
@@ -25265,7 +25268,7 @@
         <v>69</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>149</v>
@@ -25307,7 +25310,7 @@
         <v>2</v>
       </c>
       <c r="Q35" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R35" s="0" t="s">
         <v>149</v>
@@ -25345,7 +25348,7 @@
         <v>70</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>149</v>
@@ -25387,7 +25390,7 @@
         <v>2</v>
       </c>
       <c r="Q36" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R36" s="0" t="s">
         <v>149</v>
@@ -25425,7 +25428,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>149</v>
@@ -25467,7 +25470,7 @@
         <v>2</v>
       </c>
       <c r="Q37" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R37" s="0" t="s">
         <v>149</v>
@@ -25505,7 +25508,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>149</v>
@@ -25547,7 +25550,7 @@
         <v>2</v>
       </c>
       <c r="Q38" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="R38" s="0" t="s">
         <v>149</v>
@@ -25585,7 +25588,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>149</v>
@@ -25627,7 +25630,7 @@
         <v>2</v>
       </c>
       <c r="Q39" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R39" s="0" t="s">
         <v>149</v>
@@ -25665,7 +25668,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>149</v>
@@ -25707,7 +25710,7 @@
         <v>2</v>
       </c>
       <c r="Q40" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R40" s="0" t="s">
         <v>149</v>
@@ -25745,7 +25748,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>149</v>
@@ -25787,7 +25790,7 @@
         <v>2</v>
       </c>
       <c r="Q41" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R41" s="0" t="s">
         <v>149</v>
@@ -25825,7 +25828,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>149</v>
@@ -25867,7 +25870,7 @@
         <v>2</v>
       </c>
       <c r="Q42" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="R42" s="0" t="s">
         <v>149</v>
@@ -25905,7 +25908,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>149</v>
@@ -25947,7 +25950,7 @@
         <v>2</v>
       </c>
       <c r="Q43" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R43" s="0" t="s">
         <v>149</v>
@@ -25985,7 +25988,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>149</v>
@@ -26027,7 +26030,7 @@
         <v>2</v>
       </c>
       <c r="Q44" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R44" s="0" t="s">
         <v>149</v>
@@ -26065,7 +26068,7 @@
         <v>79</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>149</v>
@@ -26107,7 +26110,7 @@
         <v>2</v>
       </c>
       <c r="Q45" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="R45" s="0" t="s">
         <v>149</v>
@@ -26145,7 +26148,7 @@
         <v>80</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>149</v>
@@ -26187,7 +26190,7 @@
         <v>2</v>
       </c>
       <c r="Q46" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="R46" s="0" t="s">
         <v>149</v>
@@ -26225,7 +26228,7 @@
         <v>81</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>149</v>
@@ -26267,7 +26270,7 @@
         <v>2</v>
       </c>
       <c r="Q47" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R47" s="0" t="s">
         <v>149</v>
@@ -26305,7 +26308,7 @@
         <v>82</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>149</v>
@@ -26347,7 +26350,7 @@
         <v>2</v>
       </c>
       <c r="Q48" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R48" s="0" t="s">
         <v>149</v>
@@ -26385,7 +26388,7 @@
         <v>85</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>149</v>
@@ -26427,7 +26430,7 @@
         <v>2</v>
       </c>
       <c r="Q49" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R49" s="0" t="s">
         <v>149</v>
@@ -26465,7 +26468,7 @@
         <v>86</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>149</v>
@@ -26507,7 +26510,7 @@
         <v>2</v>
       </c>
       <c r="Q50" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R50" s="0" t="s">
         <v>149</v>
@@ -26545,7 +26548,7 @@
         <v>88</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>149</v>
@@ -26587,7 +26590,7 @@
         <v>2</v>
       </c>
       <c r="Q51" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R51" s="0" t="s">
         <v>149</v>
@@ -26625,7 +26628,7 @@
         <v>89</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>149</v>
@@ -26667,7 +26670,7 @@
         <v>2</v>
       </c>
       <c r="Q52" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="R52" s="0" t="s">
         <v>149</v>
@@ -26705,7 +26708,7 @@
         <v>93</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>149</v>
@@ -26747,7 +26750,7 @@
         <v>2</v>
       </c>
       <c r="Q53" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R53" s="0" t="s">
         <v>149</v>
@@ -26785,7 +26788,7 @@
         <v>94</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>149</v>
@@ -26827,7 +26830,7 @@
         <v>2</v>
       </c>
       <c r="Q54" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R54" s="0" t="s">
         <v>149</v>
@@ -26865,7 +26868,7 @@
         <v>96</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>149</v>
@@ -26907,7 +26910,7 @@
         <v>2</v>
       </c>
       <c r="Q55" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R55" s="0" t="s">
         <v>149</v>
@@ -26945,7 +26948,7 @@
         <v>97</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>149</v>
@@ -26987,7 +26990,7 @@
         <v>2</v>
       </c>
       <c r="Q56" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="R56" s="0" t="s">
         <v>149</v>
@@ -27025,7 +27028,7 @@
         <v>42</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>149</v>
@@ -27067,7 +27070,7 @@
         <v>2</v>
       </c>
       <c r="Q57" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="R57" s="0" t="s">
         <v>149</v>
@@ -27105,7 +27108,7 @@
         <v>100</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>149</v>
@@ -27147,7 +27150,7 @@
         <v>2</v>
       </c>
       <c r="Q58" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R58" s="0" t="s">
         <v>149</v>
@@ -27185,7 +27188,7 @@
         <v>101</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>149</v>
@@ -27227,7 +27230,7 @@
         <v>2</v>
       </c>
       <c r="Q59" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="R59" s="0" t="s">
         <v>149</v>
@@ -27265,7 +27268,7 @@
         <v>104</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>149</v>
@@ -27307,7 +27310,7 @@
         <v>2</v>
       </c>
       <c r="Q60" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R60" s="0" t="s">
         <v>149</v>
@@ -27345,7 +27348,7 @@
         <v>107</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>149</v>
@@ -27387,7 +27390,7 @@
         <v>2</v>
       </c>
       <c r="Q61" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R61" s="0" t="s">
         <v>149</v>
@@ -27425,7 +27428,7 @@
         <v>108</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>149</v>
@@ -27467,7 +27470,7 @@
         <v>2</v>
       </c>
       <c r="Q62" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="R62" s="0" t="s">
         <v>149</v>
@@ -27505,7 +27508,7 @@
         <v>109</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>149</v>
@@ -27585,7 +27588,7 @@
         <v>110</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>149</v>
@@ -27627,7 +27630,7 @@
         <v>2</v>
       </c>
       <c r="Q64" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R64" s="0" t="s">
         <v>149</v>
@@ -27665,7 +27668,7 @@
         <v>111</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>149</v>
@@ -27707,7 +27710,7 @@
         <v>2</v>
       </c>
       <c r="Q65" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R65" s="0" t="s">
         <v>149</v>
@@ -27745,7 +27748,7 @@
         <v>112</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>149</v>
@@ -27787,7 +27790,7 @@
         <v>2</v>
       </c>
       <c r="Q66" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R66" s="0" t="s">
         <v>149</v>
@@ -27825,7 +27828,7 @@
         <v>113</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>149</v>
@@ -27867,7 +27870,7 @@
         <v>2</v>
       </c>
       <c r="Q67" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="R67" s="0" t="s">
         <v>149</v>
@@ -27905,7 +27908,7 @@
         <v>119</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>149</v>
@@ -27947,7 +27950,7 @@
         <v>2</v>
       </c>
       <c r="Q68" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R68" s="0" t="s">
         <v>167</v>
@@ -27985,7 +27988,7 @@
         <v>120</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>149</v>
@@ -28027,7 +28030,7 @@
         <v>2</v>
       </c>
       <c r="Q69" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R69" s="0" t="s">
         <v>167</v>
@@ -28065,7 +28068,7 @@
         <v>120</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>149</v>
@@ -28107,7 +28110,7 @@
         <v>2</v>
       </c>
       <c r="Q70" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R70" s="0" t="s">
         <v>167</v>
@@ -28145,7 +28148,7 @@
         <v>122</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>149</v>
@@ -28187,7 +28190,7 @@
         <v>2</v>
       </c>
       <c r="Q71" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R71" s="0" t="s">
         <v>167</v>
@@ -28225,7 +28228,7 @@
         <v>123</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>149</v>
@@ -28267,7 +28270,7 @@
         <v>2</v>
       </c>
       <c r="Q72" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="R72" s="0" t="s">
         <v>167</v>
@@ -28305,7 +28308,7 @@
         <v>124</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>149</v>
@@ -28347,7 +28350,7 @@
         <v>2</v>
       </c>
       <c r="Q73" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="R73" s="0" t="s">
         <v>167</v>
@@ -28385,7 +28388,7 @@
         <v>127</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>149</v>
@@ -28427,7 +28430,7 @@
         <v>2</v>
       </c>
       <c r="Q74" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R74" s="0" t="s">
         <v>167</v>
@@ -28465,7 +28468,7 @@
         <v>132</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>149</v>
@@ -28507,7 +28510,7 @@
         <v>2</v>
       </c>
       <c r="Q75" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R75" s="0" t="s">
         <v>167</v>
@@ -28545,7 +28548,7 @@
         <v>133</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>149</v>
@@ -28587,7 +28590,7 @@
         <v>2</v>
       </c>
       <c r="Q76" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="R76" s="0" t="s">
         <v>167</v>
@@ -28625,7 +28628,7 @@
         <v>134</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>149</v>
@@ -28667,7 +28670,7 @@
         <v>2</v>
       </c>
       <c r="Q77" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R77" s="0" t="s">
         <v>167</v>
@@ -28705,7 +28708,7 @@
         <v>135</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>149</v>
@@ -28747,7 +28750,7 @@
         <v>2</v>
       </c>
       <c r="Q78" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R78" s="0" t="s">
         <v>167</v>
@@ -28785,7 +28788,7 @@
         <v>136</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>149</v>
@@ -28827,7 +28830,7 @@
         <v>2</v>
       </c>
       <c r="Q79" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R79" s="0" t="s">
         <v>167</v>
@@ -28865,7 +28868,7 @@
         <v>136</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>149</v>
@@ -28907,7 +28910,7 @@
         <v>2</v>
       </c>
       <c r="Q80" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R80" s="0" t="s">
         <v>167</v>
@@ -28945,7 +28948,7 @@
         <v>137</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>149</v>
@@ -28987,7 +28990,7 @@
         <v>2</v>
       </c>
       <c r="Q81" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R81" s="0" t="s">
         <v>167</v>
@@ -29025,7 +29028,7 @@
         <v>138</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>149</v>
@@ -29067,7 +29070,7 @@
         <v>2</v>
       </c>
       <c r="Q82" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="R82" s="0" t="s">
         <v>167</v>
@@ -29105,7 +29108,7 @@
         <v>141</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>149</v>
@@ -29147,7 +29150,7 @@
         <v>2</v>
       </c>
       <c r="Q83" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="R83" s="0" t="s">
         <v>167</v>
@@ -29185,7 +29188,7 @@
         <v>142</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>149</v>
@@ -29227,7 +29230,7 @@
         <v>2</v>
       </c>
       <c r="Q84" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="R84" s="0" t="s">
         <v>167</v>
@@ -29278,7 +29281,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I17:I55 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q10 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29288,7 +29291,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>